<commit_message>
KontoAuszug 10 und weitere Barkasse Buchungen
</commit_message>
<xml_diff>
--- a/AWO_Einnahmen_Ausgaben_2018.xlsx
+++ b/AWO_Einnahmen_Ausgaben_2018.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
   <si>
     <t>T. z. g. Laune</t>
   </si>
@@ -347,13 +347,31 @@
     <t>Zinsen Awo BB</t>
   </si>
   <si>
-    <t>Telekom</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
     <t>alex</t>
+  </si>
+  <si>
+    <t>Miete Mai 2018 Stadt Wabu</t>
+  </si>
+  <si>
+    <t>Treff d.g.Laune 10.04.2018</t>
+  </si>
+  <si>
+    <t>Treff d.g.Laune 17.04.2018</t>
+  </si>
+  <si>
+    <t>Trauerfall Weingart 20.4.2018</t>
+  </si>
+  <si>
+    <t>Jubiläum Fr.Lustig 11.4.2018</t>
+  </si>
+  <si>
+    <t>Fahrtgeld Alex</t>
+  </si>
+  <si>
+    <t>Telekom April</t>
   </si>
 </sst>
 </file>
@@ -717,7 +735,127 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -1967,8 +2105,8 @@
   <dimension ref="A1:IK168"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <pane ySplit="2" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2695,11 +2833,21 @@
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="18"/>
+      <c r="A30" s="15">
+        <v>43223</v>
+      </c>
+      <c r="B30" s="16">
+        <v>27</v>
+      </c>
+      <c r="C30" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="18">
+        <v>173.9</v>
+      </c>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
@@ -2708,11 +2856,21 @@
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="18"/>
+      <c r="A31" s="15">
+        <v>43223</v>
+      </c>
+      <c r="B31" s="65">
+        <v>28</v>
+      </c>
+      <c r="C31" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="18">
+        <v>227.11</v>
+      </c>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -2721,11 +2879,21 @@
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" s="41" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="18"/>
+      <c r="A32" s="15">
+        <v>43223</v>
+      </c>
+      <c r="B32" s="16">
+        <v>29</v>
+      </c>
+      <c r="C32" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="18">
+        <v>36.200000000000003</v>
+      </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
@@ -3665,7 +3833,7 @@
       <c r="D104" s="27"/>
       <c r="E104" s="28">
         <f>SUM(E3:E103)</f>
-        <v>2322.880000000001</v>
+        <v>2760.0900000000011</v>
       </c>
       <c r="F104" s="29">
         <f>SUM(F3:F103)</f>
@@ -3708,11 +3876,11 @@
       <c r="D106" s="56"/>
       <c r="E106" s="29">
         <f>E104+Ausgaben!F170</f>
-        <v>168.6800000000012</v>
+        <v>462.98000000000138</v>
       </c>
       <c r="F106" s="29">
         <f>F104+Ausgaben!G170</f>
-        <v>1677.4500000000066</v>
+        <v>829.76000000000658</v>
       </c>
       <c r="G106" s="29">
         <f>G104+Ausgaben!H170</f>
@@ -3750,7 +3918,7 @@
       <c r="C108" s="25"/>
       <c r="D108" s="30">
         <f>SUM(E106:I106)</f>
-        <v>5925.9200000000083</v>
+        <v>5372.5300000000079</v>
       </c>
       <c r="E108" s="18"/>
       <c r="F108" s="19"/>
@@ -4544,23 +4712,38 @@
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="D108 E3:F4 G4 G3:I3 E104:I168 D103:I103 D5:G27 H4:I103 D30:G103 E28:G28 G29">
-    <cfRule type="cellIs" dxfId="11" priority="4" stopIfTrue="1" operator="lessThan">
+  <conditionalFormatting sqref="D108 E3:F4 G4 G3:I3 E104:I168 D103:I103 D5:G27 H4:I103 D33:G103 E28:G28 G29 E30:G32">
+    <cfRule type="cellIs" dxfId="35" priority="7" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="6" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:F29">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="5" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="4" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30">
+    <cfRule type="cellIs" dxfId="19" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4589,8 +4772,8 @@
   <dimension ref="A1:IM236"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
+      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5645,7 +5828,7 @@
       </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5701,7 +5884,7 @@
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5730,7 +5913,7 @@
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5759,7 +5942,7 @@
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5819,7 +6002,7 @@
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5910,7 +6093,7 @@
         <v>48</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>22</v>
@@ -5928,12 +6111,22 @@
     </row>
     <row r="51" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="49"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="20"/>
+      <c r="B51" s="15">
+        <v>43222</v>
+      </c>
+      <c r="C51" s="65">
+        <v>49</v>
+      </c>
+      <c r="D51" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="F51" s="21"/>
-      <c r="G51" s="22"/>
+      <c r="G51" s="22">
+        <v>-12</v>
+      </c>
       <c r="H51" s="22"/>
       <c r="I51" s="22"/>
       <c r="J51" s="23"/>
@@ -5943,12 +6136,22 @@
     </row>
     <row r="52" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="49"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="42"/>
-      <c r="E52" s="20"/>
+      <c r="B52" s="15">
+        <v>43223</v>
+      </c>
+      <c r="C52" s="65">
+        <v>50</v>
+      </c>
+      <c r="D52" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="F52" s="21"/>
-      <c r="G52" s="22"/>
+      <c r="G52" s="22">
+        <v>-280</v>
+      </c>
       <c r="H52" s="22"/>
       <c r="I52" s="22"/>
       <c r="J52" s="23"/>
@@ -5958,12 +6161,22 @@
     </row>
     <row r="53" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="49"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="65"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="20"/>
+      <c r="B53" s="15">
+        <v>43223</v>
+      </c>
+      <c r="C53" s="65">
+        <v>51</v>
+      </c>
+      <c r="D53" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>0</v>
+      </c>
       <c r="F53" s="21"/>
-      <c r="G53" s="22"/>
+      <c r="G53" s="22">
+        <v>-55.69</v>
+      </c>
       <c r="H53" s="22"/>
       <c r="I53" s="22"/>
       <c r="J53" s="23"/>
@@ -5973,11 +6186,21 @@
     </row>
     <row r="54" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="49"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="65"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="21"/>
+      <c r="B54" s="15">
+        <v>43223</v>
+      </c>
+      <c r="C54" s="65">
+        <v>52</v>
+      </c>
+      <c r="D54" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F54" s="21">
+        <v>-46</v>
+      </c>
       <c r="G54" s="22"/>
       <c r="H54" s="22"/>
       <c r="I54" s="22"/>
@@ -5985,14 +6208,258 @@
       <c r="K54" s="4"/>
       <c r="L54" s="2"/>
       <c r="M54" s="2"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="41"/>
+      <c r="P54" s="41"/>
+      <c r="Q54" s="41"/>
+      <c r="R54" s="41"/>
+      <c r="S54" s="41"/>
+      <c r="T54" s="41"/>
+      <c r="U54" s="41"/>
+      <c r="V54" s="41"/>
+      <c r="W54" s="41"/>
+      <c r="X54" s="41"/>
+      <c r="Y54" s="41"/>
+      <c r="Z54" s="41"/>
+      <c r="AA54" s="41"/>
+      <c r="AB54" s="41"/>
+      <c r="AC54" s="41"/>
+      <c r="AD54" s="41"/>
+      <c r="AE54" s="41"/>
+      <c r="AF54" s="41"/>
+      <c r="AG54" s="41"/>
+      <c r="AH54" s="41"/>
+      <c r="AI54" s="41"/>
+      <c r="AJ54" s="41"/>
+      <c r="AK54" s="41"/>
+      <c r="AL54" s="41"/>
+      <c r="AM54" s="41"/>
+      <c r="AN54" s="41"/>
+      <c r="AO54" s="41"/>
+      <c r="AP54" s="41"/>
+      <c r="AQ54" s="41"/>
+      <c r="AR54" s="41"/>
+      <c r="AS54" s="41"/>
+      <c r="AT54" s="41"/>
+      <c r="AU54" s="41"/>
+      <c r="AV54" s="41"/>
+      <c r="AW54" s="41"/>
+      <c r="AX54" s="41"/>
+      <c r="AY54" s="41"/>
+      <c r="AZ54" s="41"/>
+      <c r="BA54" s="41"/>
+      <c r="BB54" s="41"/>
+      <c r="BC54" s="41"/>
+      <c r="BD54" s="41"/>
+      <c r="BE54" s="41"/>
+      <c r="BF54" s="41"/>
+      <c r="BG54" s="41"/>
+      <c r="BH54" s="41"/>
+      <c r="BI54" s="41"/>
+      <c r="BJ54" s="41"/>
+      <c r="BK54" s="41"/>
+      <c r="BL54" s="41"/>
+      <c r="BM54" s="41"/>
+      <c r="BN54" s="41"/>
+      <c r="BO54" s="41"/>
+      <c r="BP54" s="41"/>
+      <c r="BQ54" s="41"/>
+      <c r="BR54" s="41"/>
+      <c r="BS54" s="41"/>
+      <c r="BT54" s="41"/>
+      <c r="BU54" s="41"/>
+      <c r="BV54" s="41"/>
+      <c r="BW54" s="41"/>
+      <c r="BX54" s="41"/>
+      <c r="BY54" s="41"/>
+      <c r="BZ54" s="41"/>
+      <c r="CA54" s="41"/>
+      <c r="CB54" s="41"/>
+      <c r="CC54" s="41"/>
+      <c r="CD54" s="41"/>
+      <c r="CE54" s="41"/>
+      <c r="CF54" s="41"/>
+      <c r="CG54" s="41"/>
+      <c r="CH54" s="41"/>
+      <c r="CI54" s="41"/>
+      <c r="CJ54" s="41"/>
+      <c r="CK54" s="41"/>
+      <c r="CL54" s="41"/>
+      <c r="CM54" s="41"/>
+      <c r="CN54" s="41"/>
+      <c r="CO54" s="41"/>
+      <c r="CP54" s="41"/>
+      <c r="CQ54" s="41"/>
+      <c r="CR54" s="41"/>
+      <c r="CS54" s="41"/>
+      <c r="CT54" s="41"/>
+      <c r="CU54" s="41"/>
+      <c r="CV54" s="41"/>
+      <c r="CW54" s="41"/>
+      <c r="CX54" s="41"/>
+      <c r="CY54" s="41"/>
+      <c r="CZ54" s="41"/>
+      <c r="DA54" s="41"/>
+      <c r="DB54" s="41"/>
+      <c r="DC54" s="41"/>
+      <c r="DD54" s="41"/>
+      <c r="DE54" s="41"/>
+      <c r="DF54" s="41"/>
+      <c r="DG54" s="41"/>
+      <c r="DH54" s="41"/>
+      <c r="DI54" s="41"/>
+      <c r="DJ54" s="41"/>
+      <c r="DK54" s="41"/>
+      <c r="DL54" s="41"/>
+      <c r="DM54" s="41"/>
+      <c r="DN54" s="41"/>
+      <c r="DO54" s="41"/>
+      <c r="DP54" s="41"/>
+      <c r="DQ54" s="41"/>
+      <c r="DR54" s="41"/>
+      <c r="DS54" s="41"/>
+      <c r="DT54" s="41"/>
+      <c r="DU54" s="41"/>
+      <c r="DV54" s="41"/>
+      <c r="DW54" s="41"/>
+      <c r="DX54" s="41"/>
+      <c r="DY54" s="41"/>
+      <c r="DZ54" s="41"/>
+      <c r="EA54" s="41"/>
+      <c r="EB54" s="41"/>
+      <c r="EC54" s="41"/>
+      <c r="ED54" s="41"/>
+      <c r="EE54" s="41"/>
+      <c r="EF54" s="41"/>
+      <c r="EG54" s="41"/>
+      <c r="EH54" s="41"/>
+      <c r="EI54" s="41"/>
+      <c r="EJ54" s="41"/>
+      <c r="EK54" s="41"/>
+      <c r="EL54" s="41"/>
+      <c r="EM54" s="41"/>
+      <c r="EN54" s="41"/>
+      <c r="EO54" s="41"/>
+      <c r="EP54" s="41"/>
+      <c r="EQ54" s="41"/>
+      <c r="ER54" s="41"/>
+      <c r="ES54" s="41"/>
+      <c r="ET54" s="41"/>
+      <c r="EU54" s="41"/>
+      <c r="EV54" s="41"/>
+      <c r="EW54" s="41"/>
+      <c r="EX54" s="41"/>
+      <c r="EY54" s="41"/>
+      <c r="EZ54" s="41"/>
+      <c r="FA54" s="41"/>
+      <c r="FB54" s="41"/>
+      <c r="FC54" s="41"/>
+      <c r="FD54" s="41"/>
+      <c r="FE54" s="41"/>
+      <c r="FF54" s="41"/>
+      <c r="FG54" s="41"/>
+      <c r="FH54" s="41"/>
+      <c r="FI54" s="41"/>
+      <c r="FJ54" s="41"/>
+      <c r="FK54" s="41"/>
+      <c r="FL54" s="41"/>
+      <c r="FM54" s="41"/>
+      <c r="FN54" s="41"/>
+      <c r="FO54" s="41"/>
+      <c r="FP54" s="41"/>
+      <c r="FQ54" s="41"/>
+      <c r="FR54" s="41"/>
+      <c r="FS54" s="41"/>
+      <c r="FT54" s="41"/>
+      <c r="FU54" s="41"/>
+      <c r="FV54" s="41"/>
+      <c r="FW54" s="41"/>
+      <c r="FX54" s="41"/>
+      <c r="FY54" s="41"/>
+      <c r="FZ54" s="41"/>
+      <c r="GA54" s="41"/>
+      <c r="GB54" s="41"/>
+      <c r="GC54" s="41"/>
+      <c r="GD54" s="41"/>
+      <c r="GE54" s="41"/>
+      <c r="GF54" s="41"/>
+      <c r="GG54" s="41"/>
+      <c r="GH54" s="41"/>
+      <c r="GI54" s="41"/>
+      <c r="GJ54" s="41"/>
+      <c r="GK54" s="41"/>
+      <c r="GL54" s="41"/>
+      <c r="GM54" s="41"/>
+      <c r="GN54" s="41"/>
+      <c r="GO54" s="41"/>
+      <c r="GP54" s="41"/>
+      <c r="GQ54" s="41"/>
+      <c r="GR54" s="41"/>
+      <c r="GS54" s="41"/>
+      <c r="GT54" s="41"/>
+      <c r="GU54" s="41"/>
+      <c r="GV54" s="41"/>
+      <c r="GW54" s="41"/>
+      <c r="GX54" s="41"/>
+      <c r="GY54" s="41"/>
+      <c r="GZ54" s="41"/>
+      <c r="HA54" s="41"/>
+      <c r="HB54" s="41"/>
+      <c r="HC54" s="41"/>
+      <c r="HD54" s="41"/>
+      <c r="HE54" s="41"/>
+      <c r="HF54" s="41"/>
+      <c r="HG54" s="41"/>
+      <c r="HH54" s="41"/>
+      <c r="HI54" s="41"/>
+      <c r="HJ54" s="41"/>
+      <c r="HK54" s="41"/>
+      <c r="HL54" s="41"/>
+      <c r="HM54" s="41"/>
+      <c r="HN54" s="41"/>
+      <c r="HO54" s="41"/>
+      <c r="HP54" s="41"/>
+      <c r="HQ54" s="41"/>
+      <c r="HR54" s="41"/>
+      <c r="HS54" s="41"/>
+      <c r="HT54" s="41"/>
+      <c r="HU54" s="41"/>
+      <c r="HV54" s="41"/>
+      <c r="HW54" s="41"/>
+      <c r="HX54" s="41"/>
+      <c r="HY54" s="41"/>
+      <c r="HZ54" s="41"/>
+      <c r="IA54" s="41"/>
+      <c r="IB54" s="41"/>
+      <c r="IC54" s="41"/>
+      <c r="ID54" s="41"/>
+      <c r="IE54" s="41"/>
+      <c r="IF54" s="41"/>
+      <c r="IG54" s="41"/>
+      <c r="IH54" s="41"/>
+      <c r="II54" s="41"/>
+      <c r="IJ54" s="41"/>
+      <c r="IK54" s="41"/>
+      <c r="IL54" s="41"/>
+      <c r="IM54" s="41"/>
     </row>
     <row r="55" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="49"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="65"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="21"/>
+      <c r="B55" s="15">
+        <v>43223</v>
+      </c>
+      <c r="C55" s="65">
+        <v>53</v>
+      </c>
+      <c r="D55" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="21">
+        <v>-46.91</v>
+      </c>
       <c r="G55" s="22"/>
       <c r="H55" s="22"/>
       <c r="I55" s="22"/>
@@ -6003,11 +6470,21 @@
     </row>
     <row r="56" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="49"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="65"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="21"/>
+      <c r="B56" s="15">
+        <v>43223</v>
+      </c>
+      <c r="C56" s="65">
+        <v>54</v>
+      </c>
+      <c r="D56" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="21">
+        <v>-25</v>
+      </c>
       <c r="G56" s="22"/>
       <c r="H56" s="22"/>
       <c r="I56" s="22"/>
@@ -6018,11 +6495,21 @@
     </row>
     <row r="57" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="49"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="65"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="21"/>
+      <c r="B57" s="15">
+        <v>43223</v>
+      </c>
+      <c r="C57" s="65">
+        <v>55</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" s="21">
+        <v>-25</v>
+      </c>
       <c r="G57" s="22"/>
       <c r="H57" s="22"/>
       <c r="I57" s="22"/>
@@ -6033,12 +6520,22 @@
     </row>
     <row r="58" spans="1:247" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="49"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="65"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="43"/>
+      <c r="B58" s="15">
+        <v>43223</v>
+      </c>
+      <c r="C58" s="65">
+        <v>56</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="F58" s="21"/>
-      <c r="G58" s="22"/>
+      <c r="G58" s="22">
+        <v>-500</v>
+      </c>
       <c r="H58" s="22"/>
       <c r="I58" s="22"/>
       <c r="J58" s="23"/>
@@ -33461,11 +33958,11 @@
       <c r="E170" s="33"/>
       <c r="F170" s="34">
         <f>SUM(F3:F169)</f>
-        <v>-2154.1999999999998</v>
+        <v>-2297.1099999999997</v>
       </c>
       <c r="G170" s="35">
         <f>SUM(G3:G169)</f>
-        <v>-1995.37</v>
+        <v>-2843.06</v>
       </c>
       <c r="H170" s="35">
         <f>SUM(H3:H169)</f>
@@ -35395,39 +35892,87 @@
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="K172 J171:J234 I171:I236 D171:H234 D106:E171 E3:E45 C106:C235 B106:B236 A3:A235 E51:E169">
-    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="lessThan">
+  <conditionalFormatting sqref="K172 J171:J234 I171:I236 D171:H234 D106:E171 E3:E45 C106:C235 B106:B236 A3:A53 E59:E169 A55:A235">
+    <cfRule type="cellIs" dxfId="31" priority="16" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46">
-    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="15" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="14" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="13" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="12" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="11" stopIfTrue="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E169">
+  <conditionalFormatting sqref="E51">
+    <cfRule type="cellIs" dxfId="25" priority="10" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="cellIs" dxfId="23" priority="9" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="cellIs" dxfId="21" priority="8" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54">
+    <cfRule type="cellIs" dxfId="15" priority="6" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54">
+    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="cellIs" dxfId="11" priority="4" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E53 E56:E169">
       <formula1>$M$1:$M$18</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E54:E55">
+      <formula1>$K$1:$K$18</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1"/>

</xml_diff>